<commit_message>
pure tension calculation complete
</commit_message>
<xml_diff>
--- a/parameter.xlsx
+++ b/parameter.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leeoy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leeoy\OneDrive\Desktop\BBDrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13422D07-D8ED-441D-A814-47BCC61F3993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E144491B-51BA-49C2-9211-6B989C8C9816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="13372" xr2:uid="{F6561CA5-0C56-49F4-BB53-DA748E3E0E83}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="13372"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="42" uniqueCount="24">
   <si>
     <t>Variable Name</t>
   </si>
@@ -89,14 +90,32 @@
     <t>Constants</t>
   </si>
   <si>
-    <t>g/cm^3</t>
+    <t>Tension_T</t>
+  </si>
+  <si>
+    <t>RimForce</t>
+  </si>
+  <si>
+    <t>N/m</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>kN/m</t>
+  </si>
+  <si>
+    <t>kN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -129,13 +148,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -154,7 +175,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -305,7 +326,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -329,9 +350,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -355,7 +376,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -390,7 +411,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -408,7 +429,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -433,7 +454,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -473,7 +494,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -525,10 +546,10 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>1.2</v>
+        <v>1400</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -571,4 +592,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="10.0703125" customWidth="true"/>
+    <col min="2" max="2" width="9.92578125" customWidth="true"/>
+    <col min="3" max="3" width="5.78515625" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="0">
+        <v>887.891240031866</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.4">
+      <c r="A2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="0">
+        <v>17004.13727052465</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>